<commit_message>
feature revisions - flagging sub to desat
</commit_message>
<xml_diff>
--- a/sample output/Aggregate.xlsx
+++ b/sample output/Aggregate.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
   <si>
     <t>night start</t>
   </si>
@@ -75,6 +75,60 @@
   </si>
   <si>
     <t>count spike desat</t>
+  </si>
+  <si>
+    <t>bounded desat count</t>
+  </si>
+  <si>
+    <t>bounded desat from subdesat count</t>
+  </si>
+  <si>
+    <t>bounded desat duration</t>
+  </si>
+  <si>
+    <t>bounded desat mean duration</t>
+  </si>
+  <si>
+    <t>bounded desat median duration</t>
+  </si>
+  <si>
+    <t>bounded subdesat count</t>
+  </si>
+  <si>
+    <t>bounded subdesat duration</t>
+  </si>
+  <si>
+    <t>bounded subdesat mean duration</t>
+  </si>
+  <si>
+    <t>bounded subdesat median duration</t>
+  </si>
+  <si>
+    <t>bounded sustained desat count</t>
+  </si>
+  <si>
+    <t>bounded sustained desat from subdesat count</t>
+  </si>
+  <si>
+    <t>bounded sustained desat duration</t>
+  </si>
+  <si>
+    <t>bounded sustained desat mean duration</t>
+  </si>
+  <si>
+    <t>bounded sustained desat median duration</t>
+  </si>
+  <si>
+    <t>bounded sustained subdesat count</t>
+  </si>
+  <si>
+    <t>bounded sustained subdesat duration</t>
+  </si>
+  <si>
+    <t>bounded sustained subdesat mean duration</t>
+  </si>
+  <si>
+    <t>bounded sustained subdesat median duration</t>
   </si>
   <si>
     <t>SB013</t>
@@ -589,13 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:38">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,10 +707,64 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2">
         <v>45532.87502314815</v>
@@ -668,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>36</v>
@@ -701,18 +809,60 @@
         <v>20</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>4</v>
+      </c>
+      <c r="AA2">
+        <v>52</v>
+      </c>
+      <c r="AB2">
+        <v>13</v>
+      </c>
+      <c r="AC2">
+        <v>13</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>4</v>
+      </c>
+      <c r="AJ2">
+        <v>132</v>
+      </c>
+      <c r="AK2">
+        <v>33</v>
+      </c>
+      <c r="AL2">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2">
         <v>45674.875</v>
@@ -724,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>128</v>
@@ -736,40 +886,94 @@
         <v>7348</v>
       </c>
       <c r="I3">
-        <v>6644</v>
+        <v>8096</v>
       </c>
       <c r="J3">
+        <v>59</v>
+      </c>
+      <c r="K3">
+        <v>137.2203389830509</v>
+      </c>
+      <c r="L3">
+        <v>41.09644670050761</v>
+      </c>
+      <c r="M3">
+        <v>9012</v>
+      </c>
+      <c r="N3">
+        <v>34</v>
+      </c>
+      <c r="O3">
+        <v>265.0588235294118</v>
+      </c>
+      <c r="P3">
+        <v>45.74619289340102</v>
+      </c>
+      <c r="Q3">
+        <v>9352</v>
+      </c>
+      <c r="R3">
+        <v>10548</v>
+      </c>
+      <c r="S3">
+        <v>11920</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>59</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>7788</v>
+      </c>
+      <c r="X3">
+        <v>132</v>
+      </c>
+      <c r="Y3">
+        <v>28</v>
+      </c>
+      <c r="Z3">
+        <v>89</v>
+      </c>
+      <c r="AA3">
+        <v>10548</v>
+      </c>
+      <c r="AB3">
+        <v>118.5168539325843</v>
+      </c>
+      <c r="AC3">
+        <v>118.5168539325843</v>
+      </c>
+      <c r="AD3">
+        <v>34</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>8620</v>
+      </c>
+      <c r="AG3">
+        <v>253.5294117647059</v>
+      </c>
+      <c r="AH3">
+        <v>60</v>
+      </c>
+      <c r="AI3">
         <v>47</v>
       </c>
-      <c r="K3">
-        <v>141.3617021276596</v>
-      </c>
-      <c r="L3">
-        <v>33.7258883248731</v>
-      </c>
-      <c r="M3">
-        <v>5876</v>
-      </c>
-      <c r="N3">
-        <v>30</v>
-      </c>
-      <c r="O3">
-        <v>195.8666666666667</v>
-      </c>
-      <c r="P3">
-        <v>29.82741116751269</v>
-      </c>
-      <c r="Q3">
-        <v>16700</v>
-      </c>
-      <c r="R3">
-        <v>16168</v>
-      </c>
-      <c r="S3">
-        <v>15328</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
+      <c r="AJ3">
+        <v>11920</v>
+      </c>
+      <c r="AK3">
+        <v>253.6170212765958</v>
+      </c>
+      <c r="AL3">
+        <v>253.6170212765958</v>
       </c>
     </row>
   </sheetData>
@@ -779,13 +983,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:38">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,10 +1047,64 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <v>45674.87503472222</v>
@@ -858,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>664</v>
@@ -891,18 +1149,60 @@
         <v>32</v>
       </c>
       <c r="R2">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>56</v>
+      </c>
+      <c r="AB2">
+        <v>28</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>80</v>
+      </c>
+      <c r="AK2">
+        <v>80</v>
+      </c>
+      <c r="AL2">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>45691.875</v>
@@ -914,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <v>2964</v>
@@ -926,40 +1226,94 @@
         <v>2464</v>
       </c>
       <c r="I3">
-        <v>2396</v>
+        <v>2548</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K3">
-        <v>599</v>
+        <v>254.8</v>
       </c>
       <c r="L3">
-        <v>9.989993328885923</v>
+        <v>10.62374916611074</v>
       </c>
       <c r="M3">
-        <v>2332</v>
+        <v>2744</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O3">
-        <v>777.3333333333334</v>
+        <v>343</v>
       </c>
       <c r="P3">
-        <v>9.723148765843897</v>
+        <v>11.44096064042695</v>
       </c>
       <c r="Q3">
-        <v>3376</v>
+        <v>912</v>
       </c>
       <c r="R3">
-        <v>2996</v>
+        <v>1408</v>
       </c>
       <c r="S3">
-        <v>2720</v>
+        <v>2340</v>
       </c>
       <c r="T3">
         <v>7</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>2548</v>
+      </c>
+      <c r="X3">
+        <v>254.8</v>
+      </c>
+      <c r="Y3">
+        <v>14</v>
+      </c>
+      <c r="Z3">
+        <v>56</v>
+      </c>
+      <c r="AA3">
+        <v>1408</v>
+      </c>
+      <c r="AB3">
+        <v>25.14285714285714</v>
+      </c>
+      <c r="AC3">
+        <v>25.14285714285714</v>
+      </c>
+      <c r="AD3">
+        <v>8</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>2744</v>
+      </c>
+      <c r="AG3">
+        <v>343</v>
+      </c>
+      <c r="AH3">
+        <v>52</v>
+      </c>
+      <c r="AI3">
+        <v>39</v>
+      </c>
+      <c r="AJ3">
+        <v>2340</v>
+      </c>
+      <c r="AK3">
+        <v>60</v>
+      </c>
+      <c r="AL3">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -969,13 +1323,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:38">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,10 +1387,64 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2">
         <v>45504.87503472222</v>
@@ -1048,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <v>1272</v>
@@ -1060,45 +1468,99 @@
         <v>1368</v>
       </c>
       <c r="I2">
-        <v>1344</v>
+        <v>1392</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2">
-        <v>448</v>
+        <v>464</v>
       </c>
       <c r="L2">
-        <v>4.481792717086835</v>
+        <v>4.641856742697079</v>
       </c>
       <c r="M2">
-        <v>1284</v>
+        <v>1452</v>
       </c>
       <c r="N2">
         <v>3</v>
       </c>
       <c r="O2">
-        <v>428</v>
+        <v>484</v>
       </c>
       <c r="P2">
-        <v>4.281712685074029</v>
+        <v>4.841936774709884</v>
       </c>
       <c r="Q2">
-        <v>1520</v>
+        <v>152</v>
       </c>
       <c r="R2">
-        <v>1480</v>
+        <v>196</v>
       </c>
       <c r="S2">
-        <v>1412</v>
+        <v>296</v>
       </c>
       <c r="T2">
         <v>5</v>
       </c>
+      <c r="U2">
+        <v>3</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1392</v>
+      </c>
+      <c r="X2">
+        <v>464</v>
+      </c>
+      <c r="Y2">
+        <v>336</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>196</v>
+      </c>
+      <c r="AB2">
+        <v>39.2</v>
+      </c>
+      <c r="AC2">
+        <v>39.2</v>
+      </c>
+      <c r="AD2">
+        <v>3</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>1452</v>
+      </c>
+      <c r="AG2">
+        <v>484</v>
+      </c>
+      <c r="AH2">
+        <v>356</v>
+      </c>
+      <c r="AI2">
+        <v>5</v>
+      </c>
+      <c r="AJ2">
+        <v>296</v>
+      </c>
+      <c r="AK2">
+        <v>59.2</v>
+      </c>
+      <c r="AL2">
+        <v>59.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2">
         <v>45663.875</v>
@@ -1110,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F3">
         <v>740</v>
@@ -1122,42 +1584,99 @@
         <v>152</v>
       </c>
       <c r="I3">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="K3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L3">
-        <v>0.1201489847410789</v>
+        <v>0.8410428931875525</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>544</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>45.33333333333334</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1.634026192478673</v>
       </c>
       <c r="Q3">
-        <v>8100</v>
+        <v>7948</v>
       </c>
       <c r="R3">
-        <v>6620</v>
+        <v>9456</v>
       </c>
       <c r="S3">
-        <v>4972</v>
+        <v>11100</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
+      <c r="U3">
+        <v>14</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>280</v>
+      </c>
+      <c r="X3">
+        <v>20</v>
+      </c>
+      <c r="Y3">
+        <v>16</v>
+      </c>
+      <c r="Z3">
+        <v>109</v>
+      </c>
+      <c r="AA3">
+        <v>9456</v>
+      </c>
+      <c r="AB3">
+        <v>86.75229357798165</v>
+      </c>
+      <c r="AC3">
+        <v>86.75229357798165</v>
+      </c>
+      <c r="AD3">
+        <v>12</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>544</v>
+      </c>
+      <c r="AG3">
+        <v>45.33333333333334</v>
+      </c>
+      <c r="AH3">
+        <v>36</v>
+      </c>
+      <c r="AI3">
+        <v>60</v>
+      </c>
+      <c r="AJ3">
+        <v>11100</v>
+      </c>
+      <c r="AK3">
+        <v>185</v>
+      </c>
+      <c r="AL3">
+        <v>185</v>
+      </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <v>45688.875</v>
@@ -1169,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>1120</v>
@@ -1181,40 +1700,94 @@
         <v>388</v>
       </c>
       <c r="I4">
-        <v>204</v>
+        <v>548</v>
       </c>
       <c r="J4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4">
-        <v>13.6</v>
+        <v>34.25</v>
       </c>
       <c r="L4">
-        <v>0.5926098071113177</v>
+        <v>1.591912619102951</v>
       </c>
       <c r="M4">
-        <v>28</v>
+        <v>800</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O4">
-        <v>9.333333333333334</v>
+        <v>80</v>
       </c>
       <c r="P4">
-        <v>0.08133860097606321</v>
+        <v>2.32396002788752</v>
       </c>
       <c r="Q4">
-        <v>4672</v>
+        <v>4284</v>
       </c>
       <c r="R4">
-        <v>4324</v>
+        <v>4752</v>
       </c>
       <c r="S4">
-        <v>3800</v>
+        <v>5360</v>
       </c>
       <c r="T4">
         <v>6</v>
+      </c>
+      <c r="U4">
+        <v>16</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>548</v>
+      </c>
+      <c r="X4">
+        <v>34.25</v>
+      </c>
+      <c r="Y4">
+        <v>26</v>
+      </c>
+      <c r="Z4">
+        <v>41</v>
+      </c>
+      <c r="AA4">
+        <v>4752</v>
+      </c>
+      <c r="AB4">
+        <v>115.9024390243902</v>
+      </c>
+      <c r="AC4">
+        <v>115.9024390243902</v>
+      </c>
+      <c r="AD4">
+        <v>10</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>800</v>
+      </c>
+      <c r="AG4">
+        <v>80</v>
+      </c>
+      <c r="AH4">
+        <v>76</v>
+      </c>
+      <c r="AI4">
+        <v>23</v>
+      </c>
+      <c r="AJ4">
+        <v>5360</v>
+      </c>
+      <c r="AK4">
+        <v>233.0434782608696</v>
+      </c>
+      <c r="AL4">
+        <v>233.0434782608696</v>
       </c>
     </row>
   </sheetData>
@@ -1224,13 +1797,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:AL34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:38">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1288,10 +1861,64 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2">
         <v>45499.87501157408</v>
@@ -1303,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F2">
         <v>412</v>
@@ -1315,42 +1942,99 @@
         <v>220</v>
       </c>
       <c r="I2">
-        <v>64</v>
+        <v>428</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="K2">
-        <v>9.142857142857142</v>
+        <v>17.12</v>
       </c>
       <c r="L2">
-        <v>0.1777975330592288</v>
+        <v>1.189021002333593</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>896</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="O2">
+        <v>40.72727272727273</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>2.489165462829203</v>
       </c>
       <c r="Q2">
-        <v>6380</v>
+        <v>6160</v>
       </c>
       <c r="R2">
-        <v>4280</v>
+        <v>8384</v>
       </c>
       <c r="S2">
-        <v>2444</v>
+        <v>11432</v>
       </c>
       <c r="T2">
         <v>8</v>
       </c>
+      <c r="U2">
+        <v>25</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>428</v>
+      </c>
+      <c r="X2">
+        <v>17.12</v>
+      </c>
+      <c r="Y2">
+        <v>12</v>
+      </c>
+      <c r="Z2">
+        <v>201</v>
+      </c>
+      <c r="AA2">
+        <v>8236</v>
+      </c>
+      <c r="AB2">
+        <v>40.97512437810946</v>
+      </c>
+      <c r="AC2">
+        <v>40.97512437810946</v>
+      </c>
+      <c r="AD2">
+        <v>22</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>896</v>
+      </c>
+      <c r="AG2">
+        <v>40.72727272727273</v>
+      </c>
+      <c r="AH2">
+        <v>36</v>
+      </c>
+      <c r="AI2">
+        <v>102</v>
+      </c>
+      <c r="AJ2">
+        <v>11240</v>
+      </c>
+      <c r="AK2">
+        <v>110.1960784313726</v>
+      </c>
+      <c r="AL2">
+        <v>110.1960784313726</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2">
         <v>45532.87501157408</v>
@@ -1362,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F3">
         <v>268</v>
@@ -1395,18 +2079,60 @@
         <v>8</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>24</v>
+      </c>
+      <c r="AB3">
+        <v>12</v>
+      </c>
+      <c r="AC3">
+        <v>12</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+      <c r="AJ3">
+        <v>64</v>
+      </c>
+      <c r="AK3">
+        <v>32</v>
+      </c>
+      <c r="AL3">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2">
         <v>45517.875</v>
@@ -1418,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F4">
         <v>8</v>
@@ -1430,45 +2156,99 @@
         <v>872</v>
       </c>
       <c r="I4">
-        <v>324</v>
+        <v>1488</v>
       </c>
       <c r="J4">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="K4">
-        <v>12</v>
+        <v>21.25714285714286</v>
       </c>
       <c r="L4">
-        <v>0.8999999999999999</v>
+        <v>4.133333333333333</v>
       </c>
       <c r="M4">
-        <v>28</v>
+        <v>2620</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="O4">
-        <v>14</v>
+        <v>56.95652173913044</v>
       </c>
       <c r="P4">
-        <v>0.07777777777777778</v>
+        <v>7.277777777777778</v>
       </c>
       <c r="Q4">
-        <v>3864</v>
+        <v>2992</v>
       </c>
       <c r="R4">
-        <v>2364</v>
+        <v>4872</v>
       </c>
       <c r="S4">
-        <v>1072</v>
+        <v>7584</v>
       </c>
       <c r="T4">
         <v>12</v>
       </c>
+      <c r="U4">
+        <v>70</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1488</v>
+      </c>
+      <c r="X4">
+        <v>21.25714285714286</v>
+      </c>
+      <c r="Y4">
+        <v>16</v>
+      </c>
+      <c r="Z4">
+        <v>177</v>
+      </c>
+      <c r="AA4">
+        <v>4872</v>
+      </c>
+      <c r="AB4">
+        <v>27.52542372881356</v>
+      </c>
+      <c r="AC4">
+        <v>27.52542372881356</v>
+      </c>
+      <c r="AD4">
+        <v>46</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>2620</v>
+      </c>
+      <c r="AG4">
+        <v>56.95652173913044</v>
+      </c>
+      <c r="AH4">
+        <v>38</v>
+      </c>
+      <c r="AI4">
+        <v>93</v>
+      </c>
+      <c r="AJ4">
+        <v>7584</v>
+      </c>
+      <c r="AK4">
+        <v>81.54838709677419</v>
+      </c>
+      <c r="AL4">
+        <v>81.54838709677419</v>
+      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2">
         <v>45520.875</v>
@@ -1480,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F5">
         <v>72</v>
@@ -1521,10 +2301,40 @@
       <c r="T5">
         <v>0</v>
       </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2">
         <v>45523.875</v>
@@ -1536,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F6">
         <v>80</v>
@@ -1548,42 +2358,99 @@
         <v>300</v>
       </c>
       <c r="I6">
-        <v>52</v>
+        <v>596</v>
       </c>
       <c r="J6">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K6">
-        <v>4.727272727272728</v>
+        <v>16.10810810810811</v>
       </c>
       <c r="L6">
-        <v>0.1444444444444444</v>
+        <v>1.655555555555556</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1136</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="O6">
+        <v>66.82352941176471</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>3.155555555555556</v>
       </c>
       <c r="Q6">
-        <v>1252</v>
+        <v>952</v>
       </c>
       <c r="R6">
-        <v>260</v>
+        <v>2048</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>3708</v>
       </c>
       <c r="T6">
         <v>19</v>
       </c>
+      <c r="U6">
+        <v>37</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>596</v>
+      </c>
+      <c r="X6">
+        <v>16.10810810810811</v>
+      </c>
+      <c r="Y6">
+        <v>16</v>
+      </c>
+      <c r="Z6">
+        <v>113</v>
+      </c>
+      <c r="AA6">
+        <v>2048</v>
+      </c>
+      <c r="AB6">
+        <v>18.12389380530973</v>
+      </c>
+      <c r="AC6">
+        <v>18.12389380530973</v>
+      </c>
+      <c r="AD6">
+        <v>17</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>1136</v>
+      </c>
+      <c r="AG6">
+        <v>66.82352941176471</v>
+      </c>
+      <c r="AH6">
+        <v>48</v>
+      </c>
+      <c r="AI6">
+        <v>55</v>
+      </c>
+      <c r="AJ6">
+        <v>3708</v>
+      </c>
+      <c r="AK6">
+        <v>67.41818181818182</v>
+      </c>
+      <c r="AL6">
+        <v>67.41818181818182</v>
+      </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2">
         <v>45586.875</v>
@@ -1595,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F7">
         <v>752</v>
@@ -1607,45 +2474,99 @@
         <v>660</v>
       </c>
       <c r="I7">
-        <v>484</v>
+        <v>844</v>
       </c>
       <c r="J7">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K7">
-        <v>40.33333333333334</v>
+        <v>44.42105263157895</v>
       </c>
       <c r="L7">
-        <v>1.344444444444445</v>
+        <v>2.344444444444445</v>
       </c>
       <c r="M7">
-        <v>300</v>
+        <v>1224</v>
       </c>
       <c r="N7">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="O7">
-        <v>60</v>
+        <v>64.42105263157895</v>
       </c>
       <c r="P7">
-        <v>0.8333333333333334</v>
+        <v>3.4</v>
       </c>
       <c r="Q7">
-        <v>1884</v>
+        <v>1224</v>
       </c>
       <c r="R7">
-        <v>1440</v>
+        <v>1804</v>
       </c>
       <c r="S7">
-        <v>892</v>
+        <v>2904</v>
       </c>
       <c r="T7">
         <v>7</v>
       </c>
+      <c r="U7">
+        <v>19</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>844</v>
+      </c>
+      <c r="X7">
+        <v>44.42105263157895</v>
+      </c>
+      <c r="Y7">
+        <v>16</v>
+      </c>
+      <c r="Z7">
+        <v>61</v>
+      </c>
+      <c r="AA7">
+        <v>1796</v>
+      </c>
+      <c r="AB7">
+        <v>29.44262295081967</v>
+      </c>
+      <c r="AC7">
+        <v>29.44262295081967</v>
+      </c>
+      <c r="AD7">
+        <v>19</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>1224</v>
+      </c>
+      <c r="AG7">
+        <v>64.42105263157895</v>
+      </c>
+      <c r="AH7">
+        <v>36</v>
+      </c>
+      <c r="AI7">
+        <v>48</v>
+      </c>
+      <c r="AJ7">
+        <v>2896</v>
+      </c>
+      <c r="AK7">
+        <v>60.33333333333334</v>
+      </c>
+      <c r="AL7">
+        <v>60.33333333333334</v>
+      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2">
         <v>45519.875</v>
@@ -1657,7 +2578,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>28</v>
@@ -1669,42 +2590,99 @@
         <v>468</v>
       </c>
       <c r="I8">
-        <v>48</v>
+        <v>1020</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="K8">
-        <v>6.857142857142857</v>
+        <v>16.19047619047619</v>
       </c>
       <c r="L8">
-        <v>0.1333333333333333</v>
+        <v>2.833333333333333</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>2120</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="O8">
+        <v>46.08695652173913</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>5.888888888888888</v>
       </c>
       <c r="Q8">
-        <v>1920</v>
+        <v>1452</v>
       </c>
       <c r="R8">
-        <v>316</v>
+        <v>3344</v>
       </c>
       <c r="S8">
-        <v>24</v>
+        <v>6424</v>
       </c>
       <c r="T8">
         <v>86</v>
       </c>
+      <c r="U8">
+        <v>63</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1020</v>
+      </c>
+      <c r="X8">
+        <v>16.19047619047619</v>
+      </c>
+      <c r="Y8">
+        <v>16</v>
+      </c>
+      <c r="Z8">
+        <v>201</v>
+      </c>
+      <c r="AA8">
+        <v>3344</v>
+      </c>
+      <c r="AB8">
+        <v>16.63681592039801</v>
+      </c>
+      <c r="AC8">
+        <v>16.63681592039801</v>
+      </c>
+      <c r="AD8">
+        <v>46</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>2120</v>
+      </c>
+      <c r="AG8">
+        <v>46.08695652173913</v>
+      </c>
+      <c r="AH8">
+        <v>36</v>
+      </c>
+      <c r="AI8">
+        <v>108</v>
+      </c>
+      <c r="AJ8">
+        <v>6424</v>
+      </c>
+      <c r="AK8">
+        <v>59.48148148148148</v>
+      </c>
+      <c r="AL8">
+        <v>59.48148148148148</v>
+      </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2">
         <v>45506.87502314815</v>
@@ -1716,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>384</v>
@@ -1757,10 +2735,40 @@
       <c r="T9">
         <v>0</v>
       </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2">
         <v>45506.87501157408</v>
@@ -1772,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F10">
         <v>76</v>
@@ -1805,18 +2813,60 @@
         <v>24</v>
       </c>
       <c r="R10">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="T10">
         <v>0</v>
       </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>32</v>
+      </c>
+      <c r="AB10">
+        <v>32</v>
+      </c>
+      <c r="AC10">
+        <v>32</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>52</v>
+      </c>
+      <c r="AK10">
+        <v>52</v>
+      </c>
+      <c r="AL10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2">
         <v>45586.875</v>
@@ -1828,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -1869,10 +2919,40 @@
       <c r="T11">
         <v>0</v>
       </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2">
         <v>45553.87503472222</v>
@@ -1884,7 +2964,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F12">
         <v>28</v>
@@ -1925,10 +3005,40 @@
       <c r="T12">
         <v>0</v>
       </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2">
         <v>45553.87501157408</v>
@@ -1940,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="F13">
         <v>13937</v>
@@ -1952,45 +3062,99 @@
         <v>704</v>
       </c>
       <c r="I13">
-        <v>644</v>
+        <v>768</v>
       </c>
       <c r="J13">
         <v>7</v>
       </c>
       <c r="K13">
-        <v>92</v>
+        <v>109.7142857142857</v>
       </c>
       <c r="L13">
-        <v>1.789037975386838</v>
+        <v>2.133511125927161</v>
       </c>
       <c r="M13">
-        <v>528</v>
+        <v>908</v>
       </c>
       <c r="N13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O13">
-        <v>105.6</v>
+        <v>129.7142857142857</v>
       </c>
       <c r="P13">
-        <v>1.466788899074923</v>
+        <v>2.5224324249243</v>
       </c>
       <c r="Q13">
-        <v>14057</v>
+        <v>13353</v>
       </c>
       <c r="R13">
-        <v>13965</v>
+        <v>13461</v>
       </c>
       <c r="S13">
-        <v>13777</v>
+        <v>13697</v>
       </c>
       <c r="T13">
         <v>17</v>
       </c>
+      <c r="U13">
+        <v>7</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>768</v>
+      </c>
+      <c r="X13">
+        <v>109.7142857142857</v>
+      </c>
+      <c r="Y13">
+        <v>44</v>
+      </c>
+      <c r="Z13">
+        <v>13</v>
+      </c>
+      <c r="AA13">
+        <v>13461</v>
+      </c>
+      <c r="AB13">
+        <v>1035.461538461539</v>
+      </c>
+      <c r="AC13">
+        <v>1035.461538461539</v>
+      </c>
+      <c r="AD13">
+        <v>7</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>908</v>
+      </c>
+      <c r="AG13">
+        <v>129.7142857142857</v>
+      </c>
+      <c r="AH13">
+        <v>64</v>
+      </c>
+      <c r="AI13">
+        <v>11</v>
+      </c>
+      <c r="AJ13">
+        <v>13697</v>
+      </c>
+      <c r="AK13">
+        <v>1245.181818181818</v>
+      </c>
+      <c r="AL13">
+        <v>1245.181818181818</v>
+      </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2">
         <v>45541.87502314815</v>
@@ -2002,7 +3166,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F14">
         <v>68</v>
@@ -2014,42 +3178,99 @@
         <v>132</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>292</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>14.6</v>
       </c>
       <c r="L14">
-        <v>0.0111123458162018</v>
+        <v>0.8112012445827315</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>676</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="O14">
+        <v>35.57894736842105</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1.877986442938104</v>
       </c>
       <c r="Q14">
-        <v>1888</v>
+        <v>1756</v>
       </c>
       <c r="R14">
-        <v>652</v>
+        <v>3152</v>
       </c>
       <c r="S14">
-        <v>204</v>
+        <v>5708</v>
       </c>
       <c r="T14">
         <v>14</v>
       </c>
+      <c r="U14">
+        <v>20</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>292</v>
+      </c>
+      <c r="X14">
+        <v>14.6</v>
+      </c>
+      <c r="Y14">
+        <v>16</v>
+      </c>
+      <c r="Z14">
+        <v>152</v>
+      </c>
+      <c r="AA14">
+        <v>3152</v>
+      </c>
+      <c r="AB14">
+        <v>20.73684210526316</v>
+      </c>
+      <c r="AC14">
+        <v>20.73684210526316</v>
+      </c>
+      <c r="AD14">
+        <v>19</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>676</v>
+      </c>
+      <c r="AG14">
+        <v>35.57894736842105</v>
+      </c>
+      <c r="AH14">
+        <v>36</v>
+      </c>
+      <c r="AI14">
+        <v>98</v>
+      </c>
+      <c r="AJ14">
+        <v>5708</v>
+      </c>
+      <c r="AK14">
+        <v>58.24489795918367</v>
+      </c>
+      <c r="AL14">
+        <v>58.24489795918367</v>
+      </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2">
         <v>45555.87503472222</v>
@@ -2061,7 +3282,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F15">
         <v>824</v>
@@ -2073,45 +3294,99 @@
         <v>832</v>
       </c>
       <c r="I15">
-        <v>548</v>
+        <v>1156</v>
       </c>
       <c r="J15">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K15">
-        <v>36.53333333333333</v>
+        <v>37.29032258064516</v>
       </c>
       <c r="L15">
-        <v>1.522391376819647</v>
+        <v>3.21146794088232</v>
       </c>
       <c r="M15">
-        <v>336</v>
+        <v>1648</v>
       </c>
       <c r="N15">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="O15">
-        <v>48</v>
+        <v>86.73684210526316</v>
       </c>
       <c r="P15">
-        <v>0.9334370485609512</v>
+        <v>4.578286476275141</v>
       </c>
       <c r="Q15">
-        <v>4304</v>
+        <v>3472</v>
       </c>
       <c r="R15">
-        <v>3892</v>
+        <v>4168</v>
       </c>
       <c r="S15">
-        <v>3516</v>
+        <v>5020</v>
       </c>
       <c r="T15">
         <v>2</v>
       </c>
+      <c r="U15">
+        <v>31</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1156</v>
+      </c>
+      <c r="X15">
+        <v>37.29032258064516</v>
+      </c>
+      <c r="Y15">
+        <v>16</v>
+      </c>
+      <c r="Z15">
+        <v>55</v>
+      </c>
+      <c r="AA15">
+        <v>4168</v>
+      </c>
+      <c r="AB15">
+        <v>75.78181818181818</v>
+      </c>
+      <c r="AC15">
+        <v>75.78181818181818</v>
+      </c>
+      <c r="AD15">
+        <v>19</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>1648</v>
+      </c>
+      <c r="AG15">
+        <v>86.73684210526316</v>
+      </c>
+      <c r="AH15">
+        <v>52</v>
+      </c>
+      <c r="AI15">
+        <v>35</v>
+      </c>
+      <c r="AJ15">
+        <v>5020</v>
+      </c>
+      <c r="AK15">
+        <v>143.4285714285714</v>
+      </c>
+      <c r="AL15">
+        <v>143.4285714285714</v>
+      </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B16" s="2">
         <v>45558.87502314815</v>
@@ -2123,7 +3398,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F16">
         <v>164</v>
@@ -2135,39 +3410,99 @@
         <v>60</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>0.388932103567063</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>296</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <v>42.28571428571428</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>0.8223135903989333</v>
       </c>
       <c r="Q16">
-        <v>6828</v>
+        <v>6768</v>
       </c>
       <c r="R16">
-        <v>5328</v>
+        <v>8268</v>
       </c>
       <c r="S16">
-        <v>3772</v>
+        <v>9956</v>
       </c>
       <c r="T16">
         <v>2</v>
       </c>
+      <c r="U16">
+        <v>10</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>140</v>
+      </c>
+      <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="Y16">
+        <v>14</v>
+      </c>
+      <c r="Z16">
+        <v>121</v>
+      </c>
+      <c r="AA16">
+        <v>8268</v>
+      </c>
+      <c r="AB16">
+        <v>68.3305785123967</v>
+      </c>
+      <c r="AC16">
+        <v>68.3305785123967</v>
+      </c>
+      <c r="AD16">
+        <v>7</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>296</v>
+      </c>
+      <c r="AG16">
+        <v>42.28571428571428</v>
+      </c>
+      <c r="AH16">
+        <v>32</v>
+      </c>
+      <c r="AI16">
+        <v>51</v>
+      </c>
+      <c r="AJ16">
+        <v>9956</v>
+      </c>
+      <c r="AK16">
+        <v>195.2156862745098</v>
+      </c>
+      <c r="AL16">
+        <v>195.2156862745098</v>
+      </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2">
         <v>45538.87503472222</v>
@@ -2179,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F17">
         <v>476</v>
@@ -2212,18 +3547,60 @@
         <v>16</v>
       </c>
       <c r="R17">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="T17">
         <v>0</v>
       </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>32</v>
+      </c>
+      <c r="AB17">
+        <v>32</v>
+      </c>
+      <c r="AC17">
+        <v>32</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>1</v>
+      </c>
+      <c r="AJ17">
+        <v>52</v>
+      </c>
+      <c r="AK17">
+        <v>52</v>
+      </c>
+      <c r="AL17">
+        <v>52</v>
+      </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2">
         <v>45555.875</v>
@@ -2235,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F18">
         <v>36</v>
@@ -2276,10 +3653,40 @@
       <c r="T18">
         <v>0</v>
       </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2">
         <v>45561.87502314815</v>
@@ -2291,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F19">
         <v>56</v>
@@ -2324,18 +3731,60 @@
         <v>108</v>
       </c>
       <c r="R19">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>472</v>
       </c>
       <c r="T19">
         <v>1</v>
       </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>13</v>
+      </c>
+      <c r="AA19">
+        <v>212</v>
+      </c>
+      <c r="AB19">
+        <v>16.30769230769231</v>
+      </c>
+      <c r="AC19">
+        <v>16.30769230769231</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>13</v>
+      </c>
+      <c r="AJ19">
+        <v>472</v>
+      </c>
+      <c r="AK19">
+        <v>36.30769230769231</v>
+      </c>
+      <c r="AL19">
+        <v>36.30769230769231</v>
+      </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:38">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2">
         <v>45579.87502314815</v>
@@ -2347,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F20">
         <v>32</v>
@@ -2359,42 +3808,99 @@
         <v>304</v>
       </c>
       <c r="I20">
-        <v>52</v>
+        <v>608</v>
       </c>
       <c r="J20">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="K20">
-        <v>6.5</v>
+        <v>16.88888888888889</v>
       </c>
       <c r="L20">
-        <v>0.1444604956106234</v>
+        <v>1.689076564062674</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1224</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="O20">
+        <v>47.07692307692308</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>3.400377819757751</v>
       </c>
       <c r="Q20">
-        <v>1224</v>
+        <v>920</v>
       </c>
       <c r="R20">
-        <v>676</v>
+        <v>1476</v>
       </c>
       <c r="S20">
-        <v>380</v>
+        <v>2464</v>
       </c>
       <c r="T20">
         <v>28</v>
       </c>
+      <c r="U20">
+        <v>36</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>608</v>
+      </c>
+      <c r="X20">
+        <v>16.88888888888889</v>
+      </c>
+      <c r="Y20">
+        <v>16</v>
+      </c>
+      <c r="Z20">
+        <v>58</v>
+      </c>
+      <c r="AA20">
+        <v>1476</v>
+      </c>
+      <c r="AB20">
+        <v>25.44827586206896</v>
+      </c>
+      <c r="AC20">
+        <v>25.44827586206896</v>
+      </c>
+      <c r="AD20">
+        <v>26</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>1224</v>
+      </c>
+      <c r="AG20">
+        <v>47.07692307692308</v>
+      </c>
+      <c r="AH20">
+        <v>40</v>
+      </c>
+      <c r="AI20">
+        <v>38</v>
+      </c>
+      <c r="AJ20">
+        <v>2464</v>
+      </c>
+      <c r="AK20">
+        <v>64.84210526315789</v>
+      </c>
+      <c r="AL20">
+        <v>64.84210526315789</v>
+      </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2">
         <v>45587.87501157408</v>
@@ -2406,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F21">
         <v>100</v>
@@ -2418,45 +3924,99 @@
         <v>960</v>
       </c>
       <c r="I21">
-        <v>416</v>
+        <v>1580</v>
       </c>
       <c r="J21">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="K21">
-        <v>13.41935483870968</v>
+        <v>24.30769230769231</v>
       </c>
       <c r="L21">
-        <v>1.155683964884987</v>
+        <v>4.389376597399711</v>
       </c>
       <c r="M21">
-        <v>84</v>
+        <v>2660</v>
       </c>
       <c r="N21">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="O21">
-        <v>21</v>
+        <v>63.33333333333334</v>
       </c>
       <c r="P21">
-        <v>0.2333592621402378</v>
+        <v>7.389709967774197</v>
       </c>
       <c r="Q21">
-        <v>10768</v>
+        <v>9808</v>
       </c>
       <c r="R21">
-        <v>7956</v>
+        <v>12888</v>
       </c>
       <c r="S21">
-        <v>5036</v>
+        <v>16636</v>
       </c>
       <c r="T21">
         <v>21</v>
       </c>
+      <c r="U21">
+        <v>65</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>1580</v>
+      </c>
+      <c r="X21">
+        <v>24.30769230769231</v>
+      </c>
+      <c r="Y21">
+        <v>16</v>
+      </c>
+      <c r="Z21">
+        <v>265</v>
+      </c>
+      <c r="AA21">
+        <v>12820</v>
+      </c>
+      <c r="AB21">
+        <v>48.37735849056604</v>
+      </c>
+      <c r="AC21">
+        <v>48.37735849056604</v>
+      </c>
+      <c r="AD21">
+        <v>42</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>2660</v>
+      </c>
+      <c r="AG21">
+        <v>63.33333333333334</v>
+      </c>
+      <c r="AH21">
+        <v>36</v>
+      </c>
+      <c r="AI21">
+        <v>125</v>
+      </c>
+      <c r="AJ21">
+        <v>16280</v>
+      </c>
+      <c r="AK21">
+        <v>130.24</v>
+      </c>
+      <c r="AL21">
+        <v>130.24</v>
+      </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2">
         <v>45588.87501157408</v>
@@ -2468,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F22">
         <v>296</v>
@@ -2480,45 +4040,99 @@
         <v>68</v>
       </c>
       <c r="I22">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K22">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L22">
-        <v>0.111123458162018</v>
+        <v>0.277808645405045</v>
       </c>
       <c r="M22">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O22">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="P22">
-        <v>0.0333370374486054</v>
+        <v>0.5000555617290809</v>
       </c>
       <c r="Q22">
-        <v>3552</v>
+        <v>3484</v>
       </c>
       <c r="R22">
-        <v>2140</v>
+        <v>4936</v>
       </c>
       <c r="S22">
-        <v>1040</v>
+        <v>7220</v>
       </c>
       <c r="T22">
         <v>1</v>
       </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>100</v>
+      </c>
+      <c r="X22">
+        <v>25</v>
+      </c>
+      <c r="Y22">
+        <v>20</v>
+      </c>
+      <c r="Z22">
+        <v>138</v>
+      </c>
+      <c r="AA22">
+        <v>4936</v>
+      </c>
+      <c r="AB22">
+        <v>35.76811594202898</v>
+      </c>
+      <c r="AC22">
+        <v>35.76811594202898</v>
+      </c>
+      <c r="AD22">
+        <v>4</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>180</v>
+      </c>
+      <c r="AG22">
+        <v>45</v>
+      </c>
+      <c r="AH22">
+        <v>40</v>
+      </c>
+      <c r="AI22">
+        <v>82</v>
+      </c>
+      <c r="AJ22">
+        <v>7220</v>
+      </c>
+      <c r="AK22">
+        <v>88.04878048780488</v>
+      </c>
+      <c r="AL22">
+        <v>88.04878048780488</v>
+      </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2">
         <v>45589.87503472222</v>
@@ -2530,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F23">
         <v>164</v>
@@ -2542,45 +4156,99 @@
         <v>6680</v>
       </c>
       <c r="I23">
-        <v>5612</v>
+        <v>7688</v>
       </c>
       <c r="J23">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K23">
-        <v>63.0561797752809</v>
+        <v>85.42222222222222</v>
       </c>
       <c r="L23">
-        <v>15.59062118013113</v>
+        <v>21.35792865873986</v>
       </c>
       <c r="M23">
-        <v>4276</v>
+        <v>8968</v>
       </c>
       <c r="N23">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O23">
-        <v>99.44186046511628</v>
+        <v>190.8085106382979</v>
       </c>
       <c r="P23">
-        <v>11.87909767751973</v>
+        <v>24.91387931992444</v>
       </c>
       <c r="Q23">
-        <v>16712</v>
+        <v>10032</v>
       </c>
       <c r="R23">
-        <v>15172</v>
+        <v>12592</v>
       </c>
       <c r="S23">
-        <v>13240</v>
+        <v>15836</v>
       </c>
       <c r="T23">
         <v>1</v>
       </c>
+      <c r="U23">
+        <v>90</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>7688</v>
+      </c>
+      <c r="X23">
+        <v>85.42222222222222</v>
+      </c>
+      <c r="Y23">
+        <v>22</v>
+      </c>
+      <c r="Z23">
+        <v>217</v>
+      </c>
+      <c r="AA23">
+        <v>12592</v>
+      </c>
+      <c r="AB23">
+        <v>58.02764976958525</v>
+      </c>
+      <c r="AC23">
+        <v>58.02764976958525</v>
+      </c>
+      <c r="AD23">
+        <v>47</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>8968</v>
+      </c>
+      <c r="AG23">
+        <v>190.8085106382979</v>
+      </c>
+      <c r="AH23">
+        <v>56</v>
+      </c>
+      <c r="AI23">
+        <v>101</v>
+      </c>
+      <c r="AJ23">
+        <v>15836</v>
+      </c>
+      <c r="AK23">
+        <v>156.7920792079208</v>
+      </c>
+      <c r="AL23">
+        <v>156.7920792079208</v>
+      </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:38">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2">
         <v>45622.87502314815</v>
@@ -2592,7 +4260,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F24">
         <v>40</v>
@@ -2604,45 +4272,99 @@
         <v>5032</v>
       </c>
       <c r="I24">
-        <v>3412</v>
+        <v>6652</v>
       </c>
       <c r="J24">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="K24">
-        <v>31.30275229357798</v>
+        <v>56.85470085470085</v>
       </c>
       <c r="L24">
-        <v>9.478830981220135</v>
+        <v>18.47983109234359</v>
       </c>
       <c r="M24">
-        <v>2032</v>
+        <v>8428</v>
       </c>
       <c r="N24">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="O24">
-        <v>56.44444444444444</v>
+        <v>140.4666666666667</v>
       </c>
       <c r="P24">
-        <v>5.645071674630515</v>
+        <v>23.41371263473719</v>
       </c>
       <c r="Q24">
-        <v>15536</v>
+        <v>10504</v>
       </c>
       <c r="R24">
-        <v>14252</v>
+        <v>13272</v>
       </c>
       <c r="S24">
-        <v>12760</v>
+        <v>15832</v>
       </c>
       <c r="T24">
         <v>1</v>
       </c>
+      <c r="U24">
+        <v>117</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>6652</v>
+      </c>
+      <c r="X24">
+        <v>56.85470085470085</v>
+      </c>
+      <c r="Y24">
+        <v>24</v>
+      </c>
+      <c r="Z24">
+        <v>191</v>
+      </c>
+      <c r="AA24">
+        <v>13272</v>
+      </c>
+      <c r="AB24">
+        <v>69.4869109947644</v>
+      </c>
+      <c r="AC24">
+        <v>69.4869109947644</v>
+      </c>
+      <c r="AD24">
+        <v>60</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>8428</v>
+      </c>
+      <c r="AG24">
+        <v>140.4666666666667</v>
+      </c>
+      <c r="AH24">
+        <v>46</v>
+      </c>
+      <c r="AI24">
+        <v>73</v>
+      </c>
+      <c r="AJ24">
+        <v>15832</v>
+      </c>
+      <c r="AK24">
+        <v>216.8767123287671</v>
+      </c>
+      <c r="AL24">
+        <v>216.8767123287671</v>
+      </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:38">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2">
         <v>45621.87501157408</v>
@@ -2654,7 +4376,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F25">
         <v>540</v>
@@ -2666,45 +4388,99 @@
         <v>1284</v>
       </c>
       <c r="I25">
-        <v>1024</v>
+        <v>1576</v>
       </c>
       <c r="J25">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="K25">
-        <v>56.88888888888889</v>
+        <v>46.35294117647059</v>
       </c>
       <c r="L25">
-        <v>2.844760528947661</v>
+        <v>4.378264251583509</v>
       </c>
       <c r="M25">
-        <v>768</v>
+        <v>2200</v>
       </c>
       <c r="N25">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="O25">
-        <v>96</v>
+        <v>81.48148148148148</v>
       </c>
       <c r="P25">
-        <v>2.133570396710746</v>
+        <v>6.11179019891099</v>
       </c>
       <c r="Q25">
-        <v>3936</v>
+        <v>2652</v>
       </c>
       <c r="R25">
-        <v>2992</v>
+        <v>3764</v>
       </c>
       <c r="S25">
-        <v>1956</v>
+        <v>5616</v>
       </c>
       <c r="T25">
         <v>8</v>
       </c>
+      <c r="U25">
+        <v>34</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>1576</v>
+      </c>
+      <c r="X25">
+        <v>46.35294117647059</v>
+      </c>
+      <c r="Y25">
+        <v>22</v>
+      </c>
+      <c r="Z25">
+        <v>111</v>
+      </c>
+      <c r="AA25">
+        <v>3764</v>
+      </c>
+      <c r="AB25">
+        <v>33.90990990990991</v>
+      </c>
+      <c r="AC25">
+        <v>33.90990990990991</v>
+      </c>
+      <c r="AD25">
+        <v>27</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>2200</v>
+      </c>
+      <c r="AG25">
+        <v>81.48148148148148</v>
+      </c>
+      <c r="AH25">
+        <v>48</v>
+      </c>
+      <c r="AI25">
+        <v>69</v>
+      </c>
+      <c r="AJ25">
+        <v>5616</v>
+      </c>
+      <c r="AK25">
+        <v>81.39130434782609</v>
+      </c>
+      <c r="AL25">
+        <v>81.39130434782609</v>
+      </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:38">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2">
         <v>45602.87503472222</v>
@@ -2716,7 +4492,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -2757,10 +4533,40 @@
       <c r="T26">
         <v>0</v>
       </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:38">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2">
         <v>45614.87503472222</v>
@@ -2772,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F27">
         <v>16</v>
@@ -2784,42 +4590,99 @@
         <v>20</v>
       </c>
       <c r="I27">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="L27">
-        <v>0.0222246916324036</v>
+        <v>0.1000111123458162</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>38</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>0.2111345705078342</v>
       </c>
       <c r="Q27">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="R27">
-        <v>24</v>
+        <v>248</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>548</v>
       </c>
       <c r="T27">
         <v>2</v>
       </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>36</v>
+      </c>
+      <c r="X27">
+        <v>18</v>
+      </c>
+      <c r="Y27">
+        <v>18</v>
+      </c>
+      <c r="Z27">
+        <v>16</v>
+      </c>
+      <c r="AA27">
+        <v>248</v>
+      </c>
+      <c r="AB27">
+        <v>15.5</v>
+      </c>
+      <c r="AC27">
+        <v>15.5</v>
+      </c>
+      <c r="AD27">
+        <v>2</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>76</v>
+      </c>
+      <c r="AG27">
+        <v>38</v>
+      </c>
+      <c r="AH27">
+        <v>38</v>
+      </c>
+      <c r="AI27">
+        <v>13</v>
+      </c>
+      <c r="AJ27">
+        <v>548</v>
+      </c>
+      <c r="AK27">
+        <v>42.15384615384615</v>
+      </c>
+      <c r="AL27">
+        <v>42.15384615384615</v>
+      </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:38">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2">
         <v>45622.87501157408</v>
@@ -2831,7 +4694,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="F28">
         <v>1382</v>
@@ -2843,42 +4706,99 @@
         <v>1108</v>
       </c>
       <c r="I28">
-        <v>308</v>
+        <v>1988</v>
       </c>
       <c r="J28">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="K28">
-        <v>5.923076923076923</v>
+        <v>18.07272727272727</v>
       </c>
       <c r="L28">
-        <v>0.8556030890605033</v>
+        <v>5.522529029390522</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>4184</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>103</v>
+      </c>
+      <c r="O28">
+        <v>40.62135922330097</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>11.62286793710762</v>
       </c>
       <c r="Q28">
-        <v>2112</v>
+        <v>1004</v>
       </c>
       <c r="R28">
-        <v>828</v>
+        <v>2468</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>5712</v>
       </c>
       <c r="T28">
         <v>12</v>
       </c>
+      <c r="U28">
+        <v>110</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>1988</v>
+      </c>
+      <c r="X28">
+        <v>18.07272727272727</v>
+      </c>
+      <c r="Y28">
+        <v>16</v>
+      </c>
+      <c r="Z28">
+        <v>172</v>
+      </c>
+      <c r="AA28">
+        <v>2468</v>
+      </c>
+      <c r="AB28">
+        <v>14.34883720930233</v>
+      </c>
+      <c r="AC28">
+        <v>14.34883720930233</v>
+      </c>
+      <c r="AD28">
+        <v>103</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <v>4184</v>
+      </c>
+      <c r="AG28">
+        <v>40.62135922330097</v>
+      </c>
+      <c r="AH28">
+        <v>40</v>
+      </c>
+      <c r="AI28">
+        <v>141</v>
+      </c>
+      <c r="AJ28">
+        <v>5712</v>
+      </c>
+      <c r="AK28">
+        <v>40.51063829787234</v>
+      </c>
+      <c r="AL28">
+        <v>40.51063829787234</v>
+      </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:38">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2">
         <v>45614.87501157408</v>
@@ -2890,7 +4810,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F29">
         <v>40</v>
@@ -2923,18 +4843,60 @@
         <v>24</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="S29">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="T29">
         <v>0</v>
       </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>4</v>
+      </c>
+      <c r="AA29">
+        <v>56</v>
+      </c>
+      <c r="AB29">
+        <v>14</v>
+      </c>
+      <c r="AC29">
+        <v>14</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AI29">
+        <v>4</v>
+      </c>
+      <c r="AJ29">
+        <v>136</v>
+      </c>
+      <c r="AK29">
+        <v>34</v>
+      </c>
+      <c r="AL29">
+        <v>34</v>
+      </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:38">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2">
         <v>45638.87501157408</v>
@@ -2946,7 +4908,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F30">
         <v>220</v>
@@ -2979,18 +4941,60 @@
         <v>104</v>
       </c>
       <c r="R30">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="S30">
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="T30">
         <v>0</v>
       </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>9</v>
+      </c>
+      <c r="AA30">
+        <v>176</v>
+      </c>
+      <c r="AB30">
+        <v>19.55555555555556</v>
+      </c>
+      <c r="AC30">
+        <v>19.55555555555556</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <v>8</v>
+      </c>
+      <c r="AJ30">
+        <v>352</v>
+      </c>
+      <c r="AK30">
+        <v>44</v>
+      </c>
+      <c r="AL30">
+        <v>44</v>
+      </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:38">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2">
         <v>45632.875</v>
@@ -3002,7 +5006,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F31">
         <v>712</v>
@@ -3014,42 +5018,99 @@
         <v>596</v>
       </c>
       <c r="I31">
-        <v>168</v>
+        <v>1068</v>
       </c>
       <c r="J31">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="K31">
-        <v>5.793103448275862</v>
+        <v>18.10169491525424</v>
       </c>
       <c r="L31">
-        <v>0.4666666666666667</v>
+        <v>2.966666666666667</v>
       </c>
       <c r="M31">
-        <v>0</v>
+        <v>2108</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="O31">
+        <v>54.05128205128205</v>
       </c>
       <c r="P31">
-        <v>0</v>
+        <v>5.855555555555555</v>
       </c>
       <c r="Q31">
-        <v>1368</v>
+        <v>772</v>
       </c>
       <c r="R31">
-        <v>552</v>
+        <v>1632</v>
       </c>
       <c r="S31">
-        <v>0</v>
+        <v>3480</v>
       </c>
       <c r="T31">
         <v>6</v>
       </c>
+      <c r="U31">
+        <v>59</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>1068</v>
+      </c>
+      <c r="X31">
+        <v>18.10169491525424</v>
+      </c>
+      <c r="Y31">
+        <v>16</v>
+      </c>
+      <c r="Z31">
+        <v>104</v>
+      </c>
+      <c r="AA31">
+        <v>1632</v>
+      </c>
+      <c r="AB31">
+        <v>15.69230769230769</v>
+      </c>
+      <c r="AC31">
+        <v>15.69230769230769</v>
+      </c>
+      <c r="AD31">
+        <v>39</v>
+      </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <v>2108</v>
+      </c>
+      <c r="AG31">
+        <v>54.05128205128205</v>
+      </c>
+      <c r="AH31">
+        <v>40</v>
+      </c>
+      <c r="AI31">
+        <v>66</v>
+      </c>
+      <c r="AJ31">
+        <v>3480</v>
+      </c>
+      <c r="AK31">
+        <v>52.72727272727273</v>
+      </c>
+      <c r="AL31">
+        <v>52.72727272727273</v>
+      </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:38">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2">
         <v>45664.87502314815</v>
@@ -3061,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F32">
         <v>356</v>
@@ -3102,10 +5163,40 @@
       <c r="T32">
         <v>0</v>
       </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:38">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2">
         <v>45693.87502314815</v>
@@ -3117,7 +5208,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F33">
         <v>36</v>
@@ -3158,10 +5249,40 @@
       <c r="T33">
         <v>1</v>
       </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:38">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2">
         <v>45695.87503472222</v>
@@ -3173,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F34">
         <v>304</v>
@@ -3185,40 +5306,94 @@
         <v>288</v>
       </c>
       <c r="I34">
-        <v>216</v>
+        <v>364</v>
       </c>
       <c r="J34">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K34">
-        <v>43.2</v>
+        <v>45.5</v>
       </c>
       <c r="L34">
-        <v>0.6000666740748972</v>
+        <v>1.011223469274364</v>
       </c>
       <c r="M34">
-        <v>132</v>
+        <v>504</v>
       </c>
       <c r="N34">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O34">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="P34">
-        <v>0.3667074119346594</v>
+        <v>1.400155572841427</v>
       </c>
       <c r="Q34">
-        <v>564</v>
+        <v>276</v>
       </c>
       <c r="R34">
-        <v>380</v>
+        <v>520</v>
       </c>
       <c r="S34">
-        <v>244</v>
+        <v>984</v>
       </c>
       <c r="T34">
         <v>5</v>
+      </c>
+      <c r="U34">
+        <v>8</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>364</v>
+      </c>
+      <c r="X34">
+        <v>45.5</v>
+      </c>
+      <c r="Y34">
+        <v>32</v>
+      </c>
+      <c r="Z34">
+        <v>26</v>
+      </c>
+      <c r="AA34">
+        <v>496</v>
+      </c>
+      <c r="AB34">
+        <v>19.07692307692308</v>
+      </c>
+      <c r="AC34">
+        <v>19.07692307692308</v>
+      </c>
+      <c r="AD34">
+        <v>6</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>432</v>
+      </c>
+      <c r="AG34">
+        <v>72</v>
+      </c>
+      <c r="AH34">
+        <v>42</v>
+      </c>
+      <c r="AI34">
+        <v>19</v>
+      </c>
+      <c r="AJ34">
+        <v>960</v>
+      </c>
+      <c r="AK34">
+        <v>50.52631578947368</v>
+      </c>
+      <c r="AL34">
+        <v>50.52631578947368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>